<commit_message>
Mise à jour de mon journal de travail.
Oubliez pas de tenir les votres à jour! ;D
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Benoît/Journal_Travail.xlsx
+++ b/Dossiers personnels/Benoît/Journal_Travail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F195762-5B3D-684A-BA0C-32E0E8B6AC79}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEB185E-F5E8-CC42-B8D7-015E331EED0C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>Amélioration du cahier des charges et du Gantt</t>
+  </si>
+  <si>
+    <t>Visionnage et lecture de tutos sur JavaFX</t>
+  </si>
+  <si>
+    <t>Discussion planification et organisation de groupe</t>
+  </si>
+  <si>
+    <t>Visionnage et lecture de tutos sur JavaFX et début de la création de l'interface graphique de la toolBar.</t>
+  </si>
+  <si>
+    <t>Visionnage et lecture de tutos sur JavaFX et suite de la création de l'interface graphique de la toolBar.</t>
   </si>
 </sst>
 </file>
@@ -453,7 +465,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -553,24 +565,48 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="3">
+        <v>43169</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
+      <c r="A12" s="3">
+        <v>43175</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>43176</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>43177</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
@@ -663,7 +699,7 @@
       </c>
       <c r="C32" s="9">
         <f>SUM(C5:C31)</f>
-        <v>15</v>
+        <v>27.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de l'action des boutons Nouveau, Ouvrir, Sauvegarder et Sauvergarder sous de la menuBar.
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Benoît/Journal_Travail.xlsx
+++ b/Dossiers personnels/Benoît/Journal_Travail.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEB185E-F5E8-CC42-B8D7-015E331EED0C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7007C6A-E11C-D044-8395-D1B464BC0596}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -65,6 +65,95 @@
   </si>
   <si>
     <t>Visionnage et lecture de tutos sur JavaFX et suite de la création de l'interface graphique de la toolBar.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ajout de l'action des boutons </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nouveau</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ouvrir</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sauvegarder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> et </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sauvergarder sous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -74,7 +163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +197,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -465,7 +562,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -608,10 +705,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="8"/>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>43186</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
@@ -699,7 +802,7 @@
       </c>
       <c r="C32" s="9">
         <f>SUM(C5:C31)</f>
-        <v>27.5</v>
+        <v>30.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de Xstream dans les dépendances maven
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Benoît/Journal_Travail.xlsx
+++ b/Dossiers personnels/Benoît/Journal_Travail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7007C6A-E11C-D044-8395-D1B464BC0596}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CF4D27-4705-6A4A-A4E0-108488D7A1EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Visionnage et lecture de tutos sur JavaFX</t>
-  </si>
-  <si>
-    <t>Discussion planification et organisation de groupe</t>
   </si>
   <si>
     <t>Visionnage et lecture de tutos sur JavaFX et début de la création de l'interface graphique de la toolBar.</t>
@@ -154,6 +151,12 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>Discussion, planification et organisation de groupe</t>
+  </si>
+  <si>
+    <t>Ajout du code gérant la sauvegarde et l'ouverture de fichier</t>
   </si>
 </sst>
 </file>
@@ -257,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -278,6 +281,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -677,7 +683,7 @@
         <v>43175</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C12" s="8">
         <v>1.5</v>
@@ -688,7 +694,7 @@
         <v>43176</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="8">
         <v>4</v>
@@ -699,32 +705,44 @@
         <v>43177</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <v>43186</v>
+        <v>43185</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="11">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>43185</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="8"/>
-    </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="8"/>
+      <c r="A17" s="3">
+        <v>43186</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
@@ -797,12 +815,17 @@
       <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="9">
-        <f>SUM(C5:C31)</f>
-        <v>30.5</v>
+      <c r="C33" s="9">
+        <f>SUM(C5:C32)</f>
+        <v>33.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAJ Journal de travail + modifs zoom
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Benoît/Journal_Travail.xlsx
+++ b/Dossiers personnels/Benoît/Journal_Travail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1862E406-FCFB-8A42-9A4E-85FFAB3D51C6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EEDD04-AE13-A548-9A92-0E585E031B6F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>Grosse séance de travail en groupe. Ajout Pencil et Eraser, export PNG/JPG, fusion calque. Refactoring complet du code, réorganisation des dossiers et de la structure et remaniement du modèle MVC. Réorganisation et redistribution des tâches.</t>
+  </si>
+  <si>
+    <t>Débugging Pencil et Eraser</t>
+  </si>
+  <si>
+    <t>fin débugging Pencil et Eraser</t>
+  </si>
+  <si>
+    <t>Ajout de l'outil Pipette et zoom</t>
+  </si>
+  <si>
+    <t>Suite ajout de l'outil zoom</t>
   </si>
 </sst>
 </file>
@@ -577,7 +589,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -816,24 +828,48 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="3">
+        <v>43223</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="8">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="3">
+        <v>43224</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="8">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="8"/>
+      <c r="A26" s="3">
+        <v>43225</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="3">
+        <v>43226</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
@@ -881,7 +917,7 @@
       </c>
       <c r="C36" s="9">
         <f>SUM(C5:C35)</f>
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modif hand + maj journal de travail
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Benoît/Journal_Travail.xlsx
+++ b/Dossiers personnels/Benoît/Journal_Travail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EEDD04-AE13-A548-9A92-0E585E031B6F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942DDD44-BAC6-B44D-8E00-F68A4DB62063}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>Suite ajout de l'outil zoom</t>
+  </si>
+  <si>
+    <t>Grosse séance de travail en groupe. Ajout des derniers outils manquants, nombreuses résolutions de bugs, Réorganisation et redistribution des tâches.</t>
+  </si>
+  <si>
+    <t>Suite tentative de solution pour le zoom et la main</t>
+  </si>
+  <si>
+    <t>Débugging et tentatives de solutions pour le zoom et la main</t>
   </si>
 </sst>
 </file>
@@ -589,7 +598,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -871,25 +880,49 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="8"/>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>43230</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>43231</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="8"/>
+      <c r="A30" s="3">
+        <v>43232</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="8"/>
+      <c r="A31" s="3">
+        <v>43233</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
@@ -917,7 +950,7 @@
       </c>
       <c r="C36" s="9">
         <f>SUM(C5:C35)</f>
-        <v>70</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin refactoring et Javadoc WindowsNewProject
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Benoît/Journal_Travail.xlsx
+++ b/Dossiers personnels/Benoît/Journal_Travail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A12FA63-0BA8-A045-B27F-A21213DA9043}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67DB4D2-3A71-9B41-9F08-32438B4FE57C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Début d'un gros refactoring de l'entierté du code</t>
+  </si>
+  <si>
+    <t>Suite refactoring et débugging</t>
   </si>
 </sst>
 </file>
@@ -600,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -939,9 +942,15 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="8"/>
+      <c r="A33" s="3">
+        <v>43236</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="8">
+        <v>12</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
@@ -959,7 +968,7 @@
       </c>
       <c r="C36" s="9">
         <f>SUM(C5:C35)</f>
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring et javadoc des classes Crop, Hand, Move, ParamCropController et ParamTextController!
Ca sera tout pour ce soir...! ^^
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Benoît/Journal_Travail.xlsx
+++ b/Dossiers personnels/Benoît/Journal_Travail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67DB4D2-3A71-9B41-9F08-32438B4FE57C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01550CC2-9552-A848-BFC1-41359611FBB8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -604,7 +604,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -953,14 +953,26 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="8"/>
+      <c r="A34" s="3">
+        <v>43237</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="8">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="8"/>
+      <c r="A35" s="3">
+        <v>43238</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="10">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
@@ -968,7 +980,7 @@
       </c>
       <c r="C36" s="9">
         <f>SUM(C5:C35)</f>
-        <v>117</v>
+        <v>130.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add CSS pour voir l'outil sélectionné + maj journal de travail
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Benoît/Journal_Travail.xlsx
+++ b/Dossiers personnels/Benoît/Journal_Travail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01550CC2-9552-A848-BFC1-41359611FBB8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A061B4E-E922-9E4D-8221-81A4C5E813AF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -189,10 +189,10 @@
     <t>Débugging et tentatives de solutions pour le zoom et la main</t>
   </si>
   <si>
-    <t>Début d'un gros refactoring de l'entierté du code</t>
-  </si>
-  <si>
-    <t>Suite refactoring et débugging</t>
+    <t>Début d'un gros refactoring de l'entierté du code + Javadoc</t>
+  </si>
+  <si>
+    <t>Suite refactoring et débugging et Javadoc</t>
   </si>
 </sst>
 </file>
@@ -601,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -970,17 +970,42 @@
       <c r="B35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="10">
-        <v>1.5</v>
+      <c r="C35" s="8">
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="3">
+        <v>43239</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>43240</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="9">
-        <f>SUM(C5:C35)</f>
-        <v>130.5</v>
+      <c r="C39" s="9">
+        <f>SUM(C5:C38)</f>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>